<commit_message>
Cambios de business intelligence
</commit_message>
<xml_diff>
--- a/Cursos/CURSO DE BUSINESS INTELLIGENCE UTILIDAD Y AREAS DE OPORTUNIDAD/08-caso-practico-1-ejercicio_43ed5970-c1bf-4691-ac5d-3dc893ec7d8a.xlsx
+++ b/Cursos/CURSO DE BUSINESS INTELLIGENCE UTILIDAD Y AREAS DE OPORTUNIDAD/08-caso-practico-1-ejercicio_43ed5970-c1bf-4691-ac5d-3dc893ec7d8a.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Vargas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\PLATZI\Cursos\CURSO DE BUSINESS INTELLIGENCE UTILIDAD Y AREAS DE OPORTUNIDAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F236A307-6303-42A1-82BD-8DF1CCB83D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF54084F-F00C-4B68-B3CF-3BA5CD78AE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22500" yWindow="2760" windowWidth="12240" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caso" sheetId="1" r:id="rId1"/>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>